<commit_message>
Update: History saved on excel files
</commit_message>
<xml_diff>
--- a/inventory-system/current_stocks.xlsx
+++ b/inventory-system/current_stocks.xlsx
@@ -425,7 +425,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:D29"/>
+  <dimension ref="A1:D30"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -458,14 +458,14 @@
     <row r="2">
       <c r="A2" t="inlineStr">
         <is>
-          <t>ALFONSO 50cl</t>
+          <t>'</t>
         </is>
       </c>
       <c r="B2" t="n">
-        <v>41</v>
+        <v>72</v>
       </c>
       <c r="C2" t="n">
-        <v>6</v>
+        <v>5</v>
       </c>
       <c r="D2" t="n">
         <v>12</v>
@@ -474,14 +474,14 @@
     <row r="3">
       <c r="A3" t="inlineStr">
         <is>
-          <t>ALFONSO 70cl</t>
+          <t>ALFONSO 50cl</t>
         </is>
       </c>
       <c r="B3" t="n">
-        <v>41</v>
+        <v>23</v>
       </c>
       <c r="C3" t="n">
-        <v>5</v>
+        <v>11</v>
       </c>
       <c r="D3" t="n">
         <v>12</v>
@@ -490,14 +490,14 @@
     <row r="4">
       <c r="A4" t="inlineStr">
         <is>
-          <t>ALFONSO 1.75</t>
+          <t>ALFONSO 70cl</t>
         </is>
       </c>
       <c r="B4" t="n">
-        <v>50</v>
+        <v>36</v>
       </c>
       <c r="C4" t="n">
-        <v>4</v>
+        <v>5</v>
       </c>
       <c r="D4" t="n">
         <v>12</v>
@@ -506,14 +506,14 @@
     <row r="5">
       <c r="A5" t="inlineStr">
         <is>
-          <t>PLATINUM 1L</t>
+          <t>ALFONSO 1.75</t>
         </is>
       </c>
       <c r="B5" t="n">
-        <v>6</v>
+        <v>32</v>
       </c>
       <c r="C5" t="n">
-        <v>3</v>
+        <v>4</v>
       </c>
       <c r="D5" t="n">
         <v>12</v>
@@ -522,14 +522,14 @@
     <row r="6">
       <c r="A6" t="inlineStr">
         <is>
-          <t>PLATINUM 1.75</t>
+          <t>PLATINUM 1L</t>
         </is>
       </c>
       <c r="B6" t="n">
-        <v>7</v>
+        <v>1</v>
       </c>
       <c r="C6" t="n">
-        <v>0</v>
+        <v>3</v>
       </c>
       <c r="D6" t="n">
         <v>12</v>
@@ -538,27 +538,27 @@
     <row r="7">
       <c r="A7" t="inlineStr">
         <is>
-          <t>ZERO</t>
+          <t>PLATINUM 1.75</t>
         </is>
       </c>
       <c r="B7" t="n">
-        <v>2</v>
+        <v>7</v>
       </c>
       <c r="C7" t="n">
         <v>0</v>
       </c>
       <c r="D7" t="n">
-        <v>6</v>
+        <v>12</v>
       </c>
     </row>
     <row r="8">
       <c r="A8" t="inlineStr">
         <is>
-          <t>ESCOBAR</t>
+          <t>ZERO</t>
         </is>
       </c>
       <c r="B8" t="n">
-        <v>55</v>
+        <v>2</v>
       </c>
       <c r="C8" t="n">
         <v>0</v>
@@ -570,30 +570,30 @@
     <row r="9">
       <c r="A9" t="inlineStr">
         <is>
-          <t>EMP 1.5</t>
+          <t>ESCOBAR</t>
         </is>
       </c>
       <c r="B9" t="n">
-        <v>3</v>
+        <v>55</v>
       </c>
       <c r="C9" t="n">
-        <v>5</v>
+        <v>0</v>
       </c>
       <c r="D9" t="n">
-        <v>12</v>
+        <v>6</v>
       </c>
     </row>
     <row r="10">
       <c r="A10" t="inlineStr">
         <is>
-          <t>EMPE 1L</t>
+          <t>EMP 1.5</t>
         </is>
       </c>
       <c r="B10" t="n">
-        <v>320</v>
+        <v>3</v>
       </c>
       <c r="C10" t="n">
-        <v>6</v>
+        <v>5</v>
       </c>
       <c r="D10" t="n">
         <v>12</v>
@@ -602,14 +602,14 @@
     <row r="11">
       <c r="A11" t="inlineStr">
         <is>
-          <t>EMPE 750</t>
+          <t>EMPE 1L</t>
         </is>
       </c>
       <c r="B11" t="n">
-        <v>5</v>
+        <v>317</v>
       </c>
       <c r="C11" t="n">
-        <v>0</v>
+        <v>6</v>
       </c>
       <c r="D11" t="n">
         <v>12</v>
@@ -618,11 +618,11 @@
     <row r="12">
       <c r="A12" t="inlineStr">
         <is>
-          <t>EMP 500ML</t>
+          <t>EMPE 750</t>
         </is>
       </c>
       <c r="B12" t="n">
-        <v>41</v>
+        <v>5</v>
       </c>
       <c r="C12" t="n">
         <v>0</v>
@@ -634,11 +634,11 @@
     <row r="13">
       <c r="A13" t="inlineStr">
         <is>
-          <t>EMPE 350</t>
+          <t>EMP 500ML</t>
         </is>
       </c>
       <c r="B13" t="n">
-        <v>18</v>
+        <v>41</v>
       </c>
       <c r="C13" t="n">
         <v>0</v>
@@ -650,27 +650,27 @@
     <row r="14">
       <c r="A14" t="inlineStr">
         <is>
-          <t>DOUBLE LIGHT 1L</t>
+          <t>EMPE 350</t>
         </is>
       </c>
       <c r="B14" t="n">
-        <v>29</v>
+        <v>18</v>
       </c>
       <c r="C14" t="n">
         <v>0</v>
       </c>
       <c r="D14" t="n">
-        <v>6</v>
+        <v>12</v>
       </c>
     </row>
     <row r="15">
       <c r="A15" t="inlineStr">
         <is>
-          <t>DOUBLE LIGHT 750</t>
+          <t>DOUBLE LIGHT 1L</t>
         </is>
       </c>
       <c r="B15" t="n">
-        <v>6</v>
+        <v>29</v>
       </c>
       <c r="C15" t="n">
         <v>0</v>
@@ -682,27 +682,27 @@
     <row r="16">
       <c r="A16" t="inlineStr">
         <is>
-          <t>GIN ROUND 350ML</t>
+          <t>DOUBLE LIGHT 750</t>
         </is>
       </c>
       <c r="B16" t="n">
-        <v>0</v>
+        <v>6</v>
       </c>
       <c r="C16" t="n">
         <v>0</v>
       </c>
       <c r="D16" t="n">
-        <v>12</v>
+        <v>6</v>
       </c>
     </row>
     <row r="17">
       <c r="A17" t="inlineStr">
         <is>
-          <t>GIN 4X4 750ML</t>
+          <t>GIN ROUND 350ML</t>
         </is>
       </c>
       <c r="B17" t="n">
-        <v>5</v>
+        <v>197</v>
       </c>
       <c r="C17" t="n">
         <v>0</v>
@@ -714,43 +714,43 @@
     <row r="18">
       <c r="A18" t="inlineStr">
         <is>
-          <t>HARI</t>
+          <t>GIN 4X4 750ML</t>
         </is>
       </c>
       <c r="B18" t="n">
-        <v>0</v>
+        <v>29</v>
       </c>
       <c r="C18" t="n">
         <v>0</v>
       </c>
       <c r="D18" t="n">
-        <v>6</v>
+        <v>12</v>
       </c>
     </row>
     <row r="19">
       <c r="A19" t="inlineStr">
         <is>
-          <t>PRIMERA 750ML</t>
+          <t>HARI</t>
         </is>
       </c>
       <c r="B19" t="n">
-        <v>10</v>
+        <v>0</v>
       </c>
       <c r="C19" t="n">
         <v>0</v>
       </c>
       <c r="D19" t="n">
-        <v>12</v>
+        <v>6</v>
       </c>
     </row>
     <row r="20">
       <c r="A20" t="inlineStr">
         <is>
-          <t>MOJITO</t>
+          <t>PRIMERA 750ML</t>
         </is>
       </c>
       <c r="B20" t="n">
-        <v>0</v>
+        <v>10</v>
       </c>
       <c r="C20" t="n">
         <v>0</v>
@@ -762,30 +762,30 @@
     <row r="21">
       <c r="A21" t="inlineStr">
         <is>
-          <t>GREEN GRAPE</t>
+          <t>MOJITO</t>
         </is>
       </c>
       <c r="B21" t="n">
-        <v>1</v>
+        <v>24</v>
       </c>
       <c r="C21" t="n">
-        <v>10</v>
+        <v>0</v>
       </c>
       <c r="D21" t="n">
-        <v>6</v>
+        <v>12</v>
       </c>
     </row>
     <row r="22">
       <c r="A22" t="inlineStr">
         <is>
-          <t>G.FRUIT</t>
+          <t>GREEN GRAPE</t>
         </is>
       </c>
       <c r="B22" t="n">
         <v>0</v>
       </c>
       <c r="C22" t="n">
-        <v>0</v>
+        <v>10</v>
       </c>
       <c r="D22" t="n">
         <v>12</v>
@@ -794,7 +794,7 @@
     <row r="23">
       <c r="A23" t="inlineStr">
         <is>
-          <t>STRAWBERRY</t>
+          <t>G.FRUIT</t>
         </is>
       </c>
       <c r="B23" t="n">
@@ -810,30 +810,30 @@
     <row r="24">
       <c r="A24" t="inlineStr">
         <is>
-          <t>FRESH</t>
+          <t>STRAWBERRY</t>
         </is>
       </c>
       <c r="B24" t="n">
-        <v>20</v>
+        <v>0</v>
       </c>
       <c r="C24" t="n">
-        <v>10</v>
+        <v>0</v>
       </c>
       <c r="D24" t="n">
-        <v>6</v>
+        <v>12</v>
       </c>
     </row>
     <row r="25">
       <c r="A25" t="inlineStr">
         <is>
-          <t>PEACH</t>
+          <t>FRESH</t>
         </is>
       </c>
       <c r="B25" t="n">
-        <v>0</v>
+        <v>20</v>
       </c>
       <c r="C25" t="n">
-        <v>0</v>
+        <v>10</v>
       </c>
       <c r="D25" t="n">
         <v>6</v>
@@ -842,7 +842,7 @@
     <row r="26">
       <c r="A26" t="inlineStr">
         <is>
-          <t>CHINGU GF</t>
+          <t>PEACH</t>
         </is>
       </c>
       <c r="B26" t="n">
@@ -852,13 +852,13 @@
         <v>0</v>
       </c>
       <c r="D26" t="n">
-        <v>12</v>
+        <v>6</v>
       </c>
     </row>
     <row r="27">
       <c r="A27" t="inlineStr">
         <is>
-          <t>SO NICE</t>
+          <t>CHINGU GF</t>
         </is>
       </c>
       <c r="B27" t="n">
@@ -868,13 +868,13 @@
         <v>0</v>
       </c>
       <c r="D27" t="n">
-        <v>6</v>
+        <v>12</v>
       </c>
     </row>
     <row r="28">
       <c r="A28" t="inlineStr">
         <is>
-          <t>FUNDADOR</t>
+          <t>SO NICE</t>
         </is>
       </c>
       <c r="B28" t="n">
@@ -884,22 +884,38 @@
         <v>0</v>
       </c>
       <c r="D28" t="n">
-        <v>12</v>
+        <v>6</v>
       </c>
     </row>
     <row r="29">
       <c r="A29" t="inlineStr">
         <is>
+          <t>FUNDADOR</t>
+        </is>
+      </c>
+      <c r="B29" t="n">
+        <v>0</v>
+      </c>
+      <c r="C29" t="n">
+        <v>0</v>
+      </c>
+      <c r="D29" t="n">
+        <v>12</v>
+      </c>
+    </row>
+    <row r="30">
+      <c r="A30" t="inlineStr">
+        <is>
           <t>KOPIKO BLANCA</t>
         </is>
       </c>
-      <c r="B29" t="n">
-        <v>0</v>
-      </c>
-      <c r="C29" t="n">
-        <v>0</v>
-      </c>
-      <c r="D29" t="n">
+      <c r="B30" t="n">
+        <v>0</v>
+      </c>
+      <c r="C30" t="n">
+        <v>0</v>
+      </c>
+      <c r="D30" t="n">
         <v>12</v>
       </c>
     </row>

</xml_diff>

<commit_message>
Fixes, Build, and Dist
Fixed layout, packaged executable, fixed negative stock value error
</commit_message>
<xml_diff>
--- a/inventory-system/current_stocks.xlsx
+++ b/inventory-system/current_stocks.xlsx
@@ -425,7 +425,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:D30"/>
+  <dimension ref="A1:D29"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -458,11 +458,11 @@
     <row r="2">
       <c r="A2" t="inlineStr">
         <is>
-          <t>'</t>
+          <t>ALFONSO 50cl</t>
         </is>
       </c>
       <c r="B2" t="n">
-        <v>72</v>
+        <v>1</v>
       </c>
       <c r="C2" t="n">
         <v>5</v>
@@ -474,14 +474,14 @@
     <row r="3">
       <c r="A3" t="inlineStr">
         <is>
-          <t>ALFONSO 50cl</t>
+          <t>ALFONSO 70cl</t>
         </is>
       </c>
       <c r="B3" t="n">
-        <v>23</v>
+        <v>1</v>
       </c>
       <c r="C3" t="n">
-        <v>11</v>
+        <v>6</v>
       </c>
       <c r="D3" t="n">
         <v>12</v>
@@ -490,14 +490,14 @@
     <row r="4">
       <c r="A4" t="inlineStr">
         <is>
-          <t>ALFONSO 70cl</t>
+          <t>ALFONSO 1.75</t>
         </is>
       </c>
       <c r="B4" t="n">
-        <v>36</v>
+        <v>43</v>
       </c>
       <c r="C4" t="n">
-        <v>5</v>
+        <v>4</v>
       </c>
       <c r="D4" t="n">
         <v>12</v>
@@ -506,14 +506,14 @@
     <row r="5">
       <c r="A5" t="inlineStr">
         <is>
-          <t>ALFONSO 1.75</t>
+          <t>PLATINUM 1L</t>
         </is>
       </c>
       <c r="B5" t="n">
-        <v>32</v>
+        <v>1</v>
       </c>
       <c r="C5" t="n">
-        <v>4</v>
+        <v>3</v>
       </c>
       <c r="D5" t="n">
         <v>12</v>
@@ -522,14 +522,14 @@
     <row r="6">
       <c r="A6" t="inlineStr">
         <is>
-          <t>PLATINUM 1L</t>
+          <t>PLATINUM 1.75</t>
         </is>
       </c>
       <c r="B6" t="n">
-        <v>1</v>
+        <v>7</v>
       </c>
       <c r="C6" t="n">
-        <v>3</v>
+        <v>0</v>
       </c>
       <c r="D6" t="n">
         <v>12</v>
@@ -538,27 +538,27 @@
     <row r="7">
       <c r="A7" t="inlineStr">
         <is>
-          <t>PLATINUM 1.75</t>
+          <t>ZERO</t>
         </is>
       </c>
       <c r="B7" t="n">
-        <v>7</v>
+        <v>2</v>
       </c>
       <c r="C7" t="n">
         <v>0</v>
       </c>
       <c r="D7" t="n">
-        <v>12</v>
+        <v>6</v>
       </c>
     </row>
     <row r="8">
       <c r="A8" t="inlineStr">
         <is>
-          <t>ZERO</t>
+          <t>ESCOBAR</t>
         </is>
       </c>
       <c r="B8" t="n">
-        <v>2</v>
+        <v>55</v>
       </c>
       <c r="C8" t="n">
         <v>0</v>
@@ -570,30 +570,30 @@
     <row r="9">
       <c r="A9" t="inlineStr">
         <is>
-          <t>ESCOBAR</t>
+          <t>EMP 1.5</t>
         </is>
       </c>
       <c r="B9" t="n">
-        <v>55</v>
+        <v>3</v>
       </c>
       <c r="C9" t="n">
-        <v>0</v>
+        <v>5</v>
       </c>
       <c r="D9" t="n">
-        <v>6</v>
+        <v>12</v>
       </c>
     </row>
     <row r="10">
       <c r="A10" t="inlineStr">
         <is>
-          <t>EMP 1.5</t>
+          <t>EMPE 1L</t>
         </is>
       </c>
       <c r="B10" t="n">
-        <v>3</v>
+        <v>320</v>
       </c>
       <c r="C10" t="n">
-        <v>5</v>
+        <v>6</v>
       </c>
       <c r="D10" t="n">
         <v>12</v>
@@ -602,14 +602,14 @@
     <row r="11">
       <c r="A11" t="inlineStr">
         <is>
-          <t>EMPE 1L</t>
+          <t>EMPE 750</t>
         </is>
       </c>
       <c r="B11" t="n">
-        <v>317</v>
+        <v>5</v>
       </c>
       <c r="C11" t="n">
-        <v>6</v>
+        <v>0</v>
       </c>
       <c r="D11" t="n">
         <v>12</v>
@@ -618,11 +618,11 @@
     <row r="12">
       <c r="A12" t="inlineStr">
         <is>
-          <t>EMPE 750</t>
+          <t>EMP 500ML</t>
         </is>
       </c>
       <c r="B12" t="n">
-        <v>5</v>
+        <v>41</v>
       </c>
       <c r="C12" t="n">
         <v>0</v>
@@ -634,11 +634,11 @@
     <row r="13">
       <c r="A13" t="inlineStr">
         <is>
-          <t>EMP 500ML</t>
+          <t>EMPE 350</t>
         </is>
       </c>
       <c r="B13" t="n">
-        <v>41</v>
+        <v>18</v>
       </c>
       <c r="C13" t="n">
         <v>0</v>
@@ -650,27 +650,27 @@
     <row r="14">
       <c r="A14" t="inlineStr">
         <is>
-          <t>EMPE 350</t>
+          <t>DOUBLE LIGHT 1L</t>
         </is>
       </c>
       <c r="B14" t="n">
-        <v>18</v>
+        <v>29</v>
       </c>
       <c r="C14" t="n">
         <v>0</v>
       </c>
       <c r="D14" t="n">
-        <v>12</v>
+        <v>6</v>
       </c>
     </row>
     <row r="15">
       <c r="A15" t="inlineStr">
         <is>
-          <t>DOUBLE LIGHT 1L</t>
+          <t>DOUBLE LIGHT 750</t>
         </is>
       </c>
       <c r="B15" t="n">
-        <v>29</v>
+        <v>6</v>
       </c>
       <c r="C15" t="n">
         <v>0</v>
@@ -682,27 +682,27 @@
     <row r="16">
       <c r="A16" t="inlineStr">
         <is>
-          <t>DOUBLE LIGHT 750</t>
+          <t>GIN ROUND 350ML</t>
         </is>
       </c>
       <c r="B16" t="n">
-        <v>6</v>
+        <v>200</v>
       </c>
       <c r="C16" t="n">
         <v>0</v>
       </c>
       <c r="D16" t="n">
-        <v>6</v>
+        <v>12</v>
       </c>
     </row>
     <row r="17">
       <c r="A17" t="inlineStr">
         <is>
-          <t>GIN ROUND 350ML</t>
+          <t>GIN 4X4 750ML</t>
         </is>
       </c>
       <c r="B17" t="n">
-        <v>197</v>
+        <v>30</v>
       </c>
       <c r="C17" t="n">
         <v>0</v>
@@ -714,43 +714,43 @@
     <row r="18">
       <c r="A18" t="inlineStr">
         <is>
-          <t>GIN 4X4 750ML</t>
+          <t>HARI</t>
         </is>
       </c>
       <c r="B18" t="n">
-        <v>29</v>
+        <v>0</v>
       </c>
       <c r="C18" t="n">
         <v>0</v>
       </c>
       <c r="D18" t="n">
-        <v>12</v>
+        <v>6</v>
       </c>
     </row>
     <row r="19">
       <c r="A19" t="inlineStr">
         <is>
-          <t>HARI</t>
+          <t>PRIMERA 750ML</t>
         </is>
       </c>
       <c r="B19" t="n">
-        <v>0</v>
+        <v>10</v>
       </c>
       <c r="C19" t="n">
         <v>0</v>
       </c>
       <c r="D19" t="n">
-        <v>6</v>
+        <v>12</v>
       </c>
     </row>
     <row r="20">
       <c r="A20" t="inlineStr">
         <is>
-          <t>PRIMERA 750ML</t>
+          <t>MOJITO</t>
         </is>
       </c>
       <c r="B20" t="n">
-        <v>10</v>
+        <v>25</v>
       </c>
       <c r="C20" t="n">
         <v>0</v>
@@ -762,14 +762,14 @@
     <row r="21">
       <c r="A21" t="inlineStr">
         <is>
-          <t>MOJITO</t>
+          <t>GREEN GRAPE</t>
         </is>
       </c>
       <c r="B21" t="n">
-        <v>24</v>
+        <v>1</v>
       </c>
       <c r="C21" t="n">
-        <v>0</v>
+        <v>10</v>
       </c>
       <c r="D21" t="n">
         <v>12</v>
@@ -778,14 +778,14 @@
     <row r="22">
       <c r="A22" t="inlineStr">
         <is>
-          <t>GREEN GRAPE</t>
+          <t>G.FRUIT</t>
         </is>
       </c>
       <c r="B22" t="n">
         <v>0</v>
       </c>
       <c r="C22" t="n">
-        <v>10</v>
+        <v>0</v>
       </c>
       <c r="D22" t="n">
         <v>12</v>
@@ -794,7 +794,7 @@
     <row r="23">
       <c r="A23" t="inlineStr">
         <is>
-          <t>G.FRUIT</t>
+          <t>STRAWBERRY</t>
         </is>
       </c>
       <c r="B23" t="n">
@@ -810,30 +810,30 @@
     <row r="24">
       <c r="A24" t="inlineStr">
         <is>
-          <t>STRAWBERRY</t>
+          <t>FRESH</t>
         </is>
       </c>
       <c r="B24" t="n">
-        <v>0</v>
+        <v>20</v>
       </c>
       <c r="C24" t="n">
-        <v>0</v>
+        <v>10</v>
       </c>
       <c r="D24" t="n">
-        <v>12</v>
+        <v>6</v>
       </c>
     </row>
     <row r="25">
       <c r="A25" t="inlineStr">
         <is>
-          <t>FRESH</t>
+          <t>PEACH</t>
         </is>
       </c>
       <c r="B25" t="n">
-        <v>20</v>
+        <v>0</v>
       </c>
       <c r="C25" t="n">
-        <v>10</v>
+        <v>0</v>
       </c>
       <c r="D25" t="n">
         <v>6</v>
@@ -842,7 +842,7 @@
     <row r="26">
       <c r="A26" t="inlineStr">
         <is>
-          <t>PEACH</t>
+          <t>CHINGU GF</t>
         </is>
       </c>
       <c r="B26" t="n">
@@ -852,13 +852,13 @@
         <v>0</v>
       </c>
       <c r="D26" t="n">
-        <v>6</v>
+        <v>12</v>
       </c>
     </row>
     <row r="27">
       <c r="A27" t="inlineStr">
         <is>
-          <t>CHINGU GF</t>
+          <t>SO NICE</t>
         </is>
       </c>
       <c r="B27" t="n">
@@ -868,13 +868,13 @@
         <v>0</v>
       </c>
       <c r="D27" t="n">
-        <v>12</v>
+        <v>6</v>
       </c>
     </row>
     <row r="28">
       <c r="A28" t="inlineStr">
         <is>
-          <t>SO NICE</t>
+          <t>FUNDADOR</t>
         </is>
       </c>
       <c r="B28" t="n">
@@ -884,13 +884,13 @@
         <v>0</v>
       </c>
       <c r="D28" t="n">
-        <v>6</v>
+        <v>12</v>
       </c>
     </row>
     <row r="29">
       <c r="A29" t="inlineStr">
         <is>
-          <t>FUNDADOR</t>
+          <t>KOPIKO BLANCA</t>
         </is>
       </c>
       <c r="B29" t="n">
@@ -900,22 +900,6 @@
         <v>0</v>
       </c>
       <c r="D29" t="n">
-        <v>12</v>
-      </c>
-    </row>
-    <row r="30">
-      <c r="A30" t="inlineStr">
-        <is>
-          <t>KOPIKO BLANCA</t>
-        </is>
-      </c>
-      <c r="B30" t="n">
-        <v>0</v>
-      </c>
-      <c r="C30" t="n">
-        <v>0</v>
-      </c>
-      <c r="D30" t="n">
         <v>12</v>
       </c>
     </row>

</xml_diff>